<commit_message>
Read and Delete Functions Broken
</commit_message>
<xml_diff>
--- a/project1/testplan.xlsx
+++ b/project1/testplan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
   <si>
     <t>Test case</t>
   </si>
@@ -81,6 +81,9 @@
     <t>Menu is displayed.</t>
   </si>
   <si>
+    <t>Menu displays correctly, if database_data does not exist, creates the file</t>
+  </si>
+  <si>
     <t>Test 2</t>
   </si>
   <si>
@@ -90,34 +93,19 @@
     <t>The program displays a message that the list is empty.</t>
   </si>
   <si>
+    <t>displays "database is empty"</t>
+  </si>
+  <si>
     <t>Test 3</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t xml:space="preserve">Select the Add Option and add the following information:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>Account#: 113344
-Name: John Smith
-Address:
-1111 Dole St.,
-Honolulu, HI 96822</t>
-    </r>
+    <t>Enter an invalid input</t>
   </si>
   <si>
-    <t xml:space="preserve">The new record is added and confirmation is displayed to the user. </t>
+    <t>The program displays a error message</t>
+  </si>
+  <si>
+    <t>displays "error: option does not exists</t>
   </si>
   <si>
     <t>Test 4</t>
@@ -139,10 +127,16 @@
         <color theme="1"/>
         <sz val="10.0"/>
       </rPr>
-      <t>Account#: 113345
+      <t>Account#: 1000
 Name: test name 1
-Address: test address at 1100 test st.</t>
+Address: test address 1</t>
     </r>
+  </si>
+  <si>
+    <t>The new record is added and confirmation is displayed to the user. Use printall to confirm</t>
+  </si>
+  <si>
+    <t>displays "The account was added succesfully", printall correctly displays address</t>
   </si>
   <si>
     <t>Test 5</t>
@@ -164,49 +158,89 @@
         <color theme="1"/>
         <sz val="10.0"/>
       </rPr>
-      <t>Account#: 112345
-Name: test name 2
-Address: test address at 1102 test st.</t>
+      <t>Account#: 1002
+Name: test name 3
+Address: test address 3</t>
     </r>
+  </si>
+  <si>
+    <t>displays "The account was added succesfully", printall correctly displays addresses in correct order</t>
   </si>
   <si>
     <t>Test 6</t>
   </si>
   <si>
-    <t>Select Find Option and input Account#: 113345</t>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t xml:space="preserve">Select the Add Option and add the following information:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>Account#: 1001
+Name: test name 2
+Address: test address 2</t>
+    </r>
+  </si>
+  <si>
+    <t>Test 7</t>
+  </si>
+  <si>
+    <t>Select Find Option and input Account#: 1000</t>
   </si>
   <si>
     <t xml:space="preserve">The record is found and confirmation is displayed to the user. </t>
   </si>
   <si>
-    <t>Test 7</t>
+    <t>The correct record is found and printed</t>
   </si>
   <si>
-    <t>Select Delete Option and delete 113345</t>
+    <t>Test 8</t>
+  </si>
+  <si>
+    <t>Select Delete Option and delete 1000</t>
   </si>
   <si>
     <t xml:space="preserve">The record is deleted and confirmation is displayed to the user. </t>
   </si>
   <si>
-    <t>Test 8</t>
+    <t>The delete option DOES NOT perform correctly, unable to properly delete function</t>
   </si>
   <si>
-    <t>Repeat Test 6</t>
+    <t xml:space="preserve"> Test 9</t>
+  </si>
+  <si>
+    <t>Repeat Test 7</t>
   </si>
   <si>
     <t xml:space="preserve">The record is not found and a error is displayed to the user. </t>
   </si>
   <si>
-    <t xml:space="preserve"> Test 9</t>
+    <t>The delete did not perform correctly, unable to test</t>
+  </si>
+  <si>
+    <t>Test 10</t>
   </si>
   <si>
     <t>Repeat Test 2</t>
   </si>
   <si>
-    <t>The program displays all records.</t>
+    <t>The program displays all records left (1002, 1001).</t>
   </si>
   <si>
-    <t>Test 10</t>
+    <t>The program correctly displays the remaining 3 since delete did not function correctly</t>
+  </si>
+  <si>
+    <t>Test 11</t>
   </si>
   <si>
     <t>Select the Quit Option</t>
@@ -214,12 +248,15 @@
   <si>
     <t>The program quits</t>
   </si>
+  <si>
+    <t>The program displays "Exiting the program..." and succesfully quits</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -242,6 +279,11 @@
       <sz val="10.0"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -312,7 +354,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -332,11 +374,17 @@
     <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
+    <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
     <xf borderId="2" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -556,7 +604,7 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="9.38"/>
     <col customWidth="1" min="2" max="3" width="32.25"/>
-    <col customWidth="1" min="4" max="4" width="21.75"/>
+    <col customWidth="1" min="4" max="4" width="41.75"/>
     <col customWidth="1" min="5" max="6" width="11.5"/>
     <col customWidth="1" min="7" max="26" width="8.63"/>
   </cols>
@@ -597,121 +645,149 @@
       <c r="C3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="6"/>
+      <c r="D3" s="7" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="4" ht="50.25" customHeight="1">
       <c r="A4" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
-      <c r="D4" s="6"/>
+      <c r="D4" s="7" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="5" ht="100.5" customHeight="1">
       <c r="A5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="6"/>
-    </row>
-    <row r="6" ht="50.25" customHeight="1">
-      <c r="A6" s="7" t="s">
+      <c r="B5" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="C5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="6"/>
-    </row>
-    <row r="7" ht="50.25" customHeight="1">
-      <c r="A7" s="7" t="s">
+      <c r="D5" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="8" t="s">
+    </row>
+    <row r="6" ht="50.25" customHeight="1">
+      <c r="A6" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="6"/>
-    </row>
-    <row r="8" ht="50.25" customHeight="1">
-      <c r="A8" s="7" t="s">
+      <c r="B6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="D6" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="6"/>
-    </row>
-    <row r="9" ht="50.25" customHeight="1">
-      <c r="A9" s="7" t="s">
+    </row>
+    <row r="7" ht="50.25" customHeight="1">
+      <c r="A7" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="6"/>
-    </row>
-    <row r="10" ht="50.25" customHeight="1">
-      <c r="A10" s="7" t="s">
+    </row>
+    <row r="8" ht="50.25" customHeight="1">
+      <c r="A8" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" ht="50.25" customHeight="1">
+      <c r="A9" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="6"/>
-    </row>
-    <row r="11" ht="50.25" customHeight="1">
-      <c r="A11" s="7" t="s">
+      <c r="B9" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="D9" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="6"/>
-    </row>
-    <row r="12" ht="50.25" customHeight="1">
-      <c r="A12" s="7" t="s">
+    </row>
+    <row r="10" ht="50.25" customHeight="1">
+      <c r="A10" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C10" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="6"/>
+      <c r="D10" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" ht="50.25" customHeight="1">
+      <c r="A11" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" ht="50.25" customHeight="1">
+      <c r="A12" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="13" ht="50.25" customHeight="1">
-      <c r="A13" s="5"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
+      <c r="A13" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="14" ht="50.25" customHeight="1">
       <c r="A14" s="5"/>

</xml_diff>